<commit_message>
Lars changes 2023-01-09 v7
</commit_message>
<xml_diff>
--- a/DO_PX/metadata/meta_BEXLTALL_Modified.xlsx
+++ b/DO_PX/metadata/meta_BEXLTALL_Modified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\STAT\GS\LARPtest\v7\DO_PX\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEEE0F2-AFAC-4F19-9E1D-6A4073A526B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C996F524-DB60-4E66-92A3-9FD738D1761D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20070" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20070" windowHeight="11850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables_MD" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="268">
   <si>
     <t>position</t>
   </si>
@@ -1220,7 +1220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -1486,8 +1486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108:E108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,6 +1531,9 @@
       <c r="E2" t="s">
         <v>26</v>
       </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1548,6 +1551,9 @@
       <c r="E3" t="s">
         <v>71</v>
       </c>
+      <c r="F3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1565,6 +1571,9 @@
       <c r="E4" t="s">
         <v>75</v>
       </c>
+      <c r="F4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1642,6 +1651,9 @@
       <c r="E8" t="s">
         <v>89</v>
       </c>
+      <c r="F8" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1659,6 +1671,9 @@
       <c r="E9" t="s">
         <v>80</v>
       </c>
+      <c r="F9" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1676,6 +1691,9 @@
       <c r="E10" t="s">
         <v>85</v>
       </c>
+      <c r="F10" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1693,6 +1711,9 @@
       <c r="E11" t="s">
         <v>87</v>
       </c>
+      <c r="F11" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1710,6 +1731,9 @@
       <c r="E12" t="s">
         <v>90</v>
       </c>
+      <c r="F12" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1727,6 +1751,9 @@
       <c r="E13" t="s">
         <v>91</v>
       </c>
+      <c r="F13" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1744,6 +1771,9 @@
       <c r="E14" t="s">
         <v>92</v>
       </c>
+      <c r="F14" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1761,6 +1791,9 @@
       <c r="E15" t="s">
         <v>93</v>
       </c>
+      <c r="F15" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1778,8 +1811,11 @@
       <c r="E16" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -1795,8 +1831,11 @@
       <c r="E17" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -1812,8 +1851,11 @@
       <c r="E18" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -1829,8 +1871,11 @@
       <c r="E19" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>88</v>
       </c>
@@ -1846,8 +1891,11 @@
       <c r="E20" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>88</v>
       </c>
@@ -1863,8 +1911,11 @@
       <c r="E21" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -1880,8 +1931,11 @@
       <c r="E22" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -1897,8 +1951,11 @@
       <c r="E23" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>88</v>
       </c>
@@ -1914,8 +1971,11 @@
       <c r="E24" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>88</v>
       </c>
@@ -1931,8 +1991,11 @@
       <c r="E25" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>88</v>
       </c>
@@ -1948,8 +2011,11 @@
       <c r="E26" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>88</v>
       </c>
@@ -1965,8 +2031,11 @@
       <c r="E27" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -1982,8 +2051,11 @@
       <c r="E28" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>88</v>
       </c>
@@ -1999,8 +2071,11 @@
       <c r="E29" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -2016,8 +2091,11 @@
       <c r="E30" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -2033,8 +2111,11 @@
       <c r="E31" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -2050,8 +2131,11 @@
       <c r="E32" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>88</v>
       </c>
@@ -2067,8 +2151,11 @@
       <c r="E33" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -2084,8 +2171,11 @@
       <c r="E34" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>88</v>
       </c>
@@ -2101,8 +2191,11 @@
       <c r="E35" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>88</v>
       </c>
@@ -2118,8 +2211,11 @@
       <c r="E36" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>88</v>
       </c>
@@ -2135,8 +2231,11 @@
       <c r="E37" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -2152,8 +2251,11 @@
       <c r="E38" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>88</v>
       </c>
@@ -2169,8 +2271,11 @@
       <c r="E39" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -2186,8 +2291,11 @@
       <c r="E40" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -2203,8 +2311,11 @@
       <c r="E41" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>88</v>
       </c>
@@ -2220,8 +2331,11 @@
       <c r="E42" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -2237,8 +2351,11 @@
       <c r="E43" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -2254,8 +2371,11 @@
       <c r="E44" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -2271,8 +2391,11 @@
       <c r="E45" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -2288,8 +2411,11 @@
       <c r="E46" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>88</v>
       </c>
@@ -2305,8 +2431,11 @@
       <c r="E47" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -2322,8 +2451,11 @@
       <c r="E48" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -2339,8 +2471,11 @@
       <c r="E49" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -2356,8 +2491,11 @@
       <c r="E50" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>88</v>
       </c>
@@ -2373,8 +2511,11 @@
       <c r="E51" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>88</v>
       </c>
@@ -2390,8 +2531,11 @@
       <c r="E52" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>88</v>
       </c>
@@ -2407,8 +2551,11 @@
       <c r="E53" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>88</v>
       </c>
@@ -2424,8 +2571,11 @@
       <c r="E54" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>88</v>
       </c>
@@ -2441,8 +2591,11 @@
       <c r="E55" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -2458,8 +2611,11 @@
       <c r="E56" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>88</v>
       </c>
@@ -2475,8 +2631,11 @@
       <c r="E57" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>88</v>
       </c>
@@ -2492,8 +2651,11 @@
       <c r="E58" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>88</v>
       </c>
@@ -2509,8 +2671,11 @@
       <c r="E59" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>88</v>
       </c>
@@ -2526,8 +2691,11 @@
       <c r="E60" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -2543,8 +2711,11 @@
       <c r="E61" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>88</v>
       </c>
@@ -2560,8 +2731,11 @@
       <c r="E62" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>88</v>
       </c>
@@ -2577,8 +2751,11 @@
       <c r="E63" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>88</v>
       </c>
@@ -2594,8 +2771,11 @@
       <c r="E64" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>88</v>
       </c>
@@ -2611,8 +2791,11 @@
       <c r="E65" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>88</v>
       </c>
@@ -2628,8 +2811,11 @@
       <c r="E66" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>88</v>
       </c>
@@ -2645,8 +2831,11 @@
       <c r="E67" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>88</v>
       </c>
@@ -2662,8 +2851,11 @@
       <c r="E68" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>88</v>
       </c>
@@ -2679,8 +2871,11 @@
       <c r="E69" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>88</v>
       </c>
@@ -2696,8 +2891,11 @@
       <c r="E70" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>88</v>
       </c>
@@ -2713,8 +2911,11 @@
       <c r="E71" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>88</v>
       </c>
@@ -2730,8 +2931,11 @@
       <c r="E72" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>88</v>
       </c>
@@ -2747,8 +2951,11 @@
       <c r="E73" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>88</v>
       </c>
@@ -2764,8 +2971,11 @@
       <c r="E74" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>88</v>
       </c>
@@ -2781,8 +2991,11 @@
       <c r="E75" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>88</v>
       </c>
@@ -2798,8 +3011,11 @@
       <c r="E76" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>88</v>
       </c>
@@ -2815,8 +3031,11 @@
       <c r="E77" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>88</v>
       </c>
@@ -2832,8 +3051,11 @@
       <c r="E78" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>88</v>
       </c>
@@ -2849,8 +3071,11 @@
       <c r="E79" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -2866,8 +3091,11 @@
       <c r="E80" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -2883,8 +3111,11 @@
       <c r="E81" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -2900,8 +3131,11 @@
       <c r="E82" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>88</v>
       </c>
@@ -2917,8 +3151,11 @@
       <c r="E83" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>88</v>
       </c>
@@ -2934,8 +3171,11 @@
       <c r="E84" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>88</v>
       </c>
@@ -2951,8 +3191,11 @@
       <c r="E85" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>88</v>
       </c>
@@ -2968,8 +3211,11 @@
       <c r="E86" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>88</v>
       </c>
@@ -2985,8 +3231,11 @@
       <c r="E87" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -3002,8 +3251,11 @@
       <c r="E88" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -3019,8 +3271,11 @@
       <c r="E89" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -3036,8 +3291,11 @@
       <c r="E90" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>88</v>
       </c>
@@ -3053,8 +3311,11 @@
       <c r="E91" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>88</v>
       </c>
@@ -3070,8 +3331,11 @@
       <c r="E92" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>88</v>
       </c>
@@ -3087,8 +3351,11 @@
       <c r="E93" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>88</v>
       </c>
@@ -3104,8 +3371,11 @@
       <c r="E94" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>88</v>
       </c>
@@ -3121,8 +3391,11 @@
       <c r="E95" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>88</v>
       </c>
@@ -3138,6 +3411,9 @@
       <c r="E96" t="s">
         <v>174</v>
       </c>
+      <c r="F96" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
@@ -3155,6 +3431,9 @@
       <c r="E97" t="s">
         <v>175</v>
       </c>
+      <c r="F97" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
@@ -3172,6 +3451,9 @@
       <c r="E98" t="s">
         <v>176</v>
       </c>
+      <c r="F98" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
@@ -3189,6 +3471,9 @@
       <c r="E99" t="s">
         <v>177</v>
       </c>
+      <c r="F99" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
@@ -3206,6 +3491,9 @@
       <c r="E100" t="s">
         <v>178</v>
       </c>
+      <c r="F100" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
@@ -3223,6 +3511,9 @@
       <c r="E101" t="s">
         <v>179</v>
       </c>
+      <c r="F101" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
@@ -3240,6 +3531,9 @@
       <c r="E102" t="s">
         <v>180</v>
       </c>
+      <c r="F102" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
@@ -3255,6 +3549,9 @@
         <v>181</v>
       </c>
       <c r="E103" t="s">
+        <v>181</v>
+      </c>
+      <c r="F103" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3274,6 +3571,9 @@
       <c r="E104" t="s">
         <v>26</v>
       </c>
+      <c r="F104" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
@@ -3291,6 +3591,9 @@
       <c r="E105" t="s">
         <v>186</v>
       </c>
+      <c r="F105" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
@@ -3307,6 +3610,9 @@
       </c>
       <c r="E106" t="s">
         <v>190</v>
+      </c>
+      <c r="F106" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>